<commit_message>
Added multiple sheet handling capability
</commit_message>
<xml_diff>
--- a/testdata/carsXlsx.xlsx
+++ b/testdata/carsXlsx.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osgoo\SBCotton\gulp-etl-tap-spreadsheet\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A018A7DE-9FDA-4776-95D7-7F0D6C6CB2D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F972F10D-5630-43D1-BEC7-14EBF47452E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-25320" yWindow="45" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cars" sheetId="1" r:id="rId1"/>
+    <sheet name="cars2" sheetId="2" r:id="rId2"/>
+    <sheet name="cars3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>carModel</t>
   </si>
@@ -53,12 +55,39 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>zcarModel</t>
+  </si>
+  <si>
+    <t>ycarModel</t>
+  </si>
+  <si>
+    <t>Chevy</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -892,10 +921,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -957,4 +988,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1118EA-44E7-41A3-A42F-2C3227FD9A8B}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>15000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>30000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5759E7-7A19-4CF9-A88A-C0FA128EB0E7}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>15000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>19000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>16000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added HTML and TXT handling
</commit_message>
<xml_diff>
--- a/testdata/carsXlsx.xlsx
+++ b/testdata/carsXlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osgoo\SBCotton\gulp-etl-tap-spreadsheet\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F972F10D-5630-43D1-BEC7-14EBF47452E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328D190B-F905-4678-86FC-A07DE326B138}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="45" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23205" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cars" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>carModel</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>black</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>Voltswagon</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Honda</t>
   </si>
 </sst>
 </file>
@@ -924,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +1010,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,32 +1028,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>15000</v>
+        <v>16000</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>20000</v>
+        <v>13000</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1046,10 +1061,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1064,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5759E7-7A19-4CF9-A88A-C0FA128EB0E7}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>